<commit_message>
- update hints and stype without affecting the data
</commit_message>
<xml_diff>
--- a/templateSampleFilled4.xlsx
+++ b/templateSampleFilled4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-contribute/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE84F79-892F-FE4A-AAD3-4D151A4ECDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90961D3-1803-E04D-B450-3E0BF26FADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="107">
   <si>
     <t>Name:</t>
   </si>
@@ -120,9 +120,6 @@
     <t>ML/EXP/EM/DFT/THM</t>
   </si>
   <si>
-    <t>Absolute Temperature</t>
-  </si>
-  <si>
     <t>Base SI Units s/Pa/m/kg</t>
   </si>
   <si>
@@ -130,6 +127,216 @@
   </si>
   <si>
     <t>phase1+phase2        no space between</t>
+  </si>
+  <si>
+    <t>id/nickname</t>
+  </si>
+  <si>
+    <t>Optional Upload Comments:</t>
+  </si>
+  <si>
+    <t>750e6</t>
+  </si>
+  <si>
+    <t>Col1</t>
+  </si>
+  <si>
+    <t>Col2</t>
+  </si>
+  <si>
+    <t>Col3</t>
+  </si>
+  <si>
+    <t>Col4</t>
+  </si>
+  <si>
+    <t>Col5</t>
+  </si>
+  <si>
+    <t>Scratch (NOT UPLOADED)</t>
+  </si>
+  <si>
+    <t>UTS in lb/in^2</t>
+  </si>
+  <si>
+    <t>Temperature in F</t>
+  </si>
+  <si>
+    <t>Some Notes</t>
+  </si>
+  <si>
+    <t>only DOI, no http etc                                                      (if no DOI) Author_Year_ThreeFirstTitleWords</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>Unit [SI]</t>
+  </si>
+  <si>
+    <t>Uncertainty in Value</t>
+  </si>
+  <si>
+    <t>25e6</t>
+  </si>
+  <si>
+    <t>Uncertainty [SI]</t>
+  </si>
+  <si>
+    <t>Special Cell</t>
+  </si>
+  <si>
+    <t>This special cell will allow running special upload functions in the future, such as (1) POSCAR, (2) TDB, (3) FIGURE, by typing the word In the cell below to engage upload script function</t>
+  </si>
+  <si>
+    <t>Property Parameters</t>
+  </si>
+  <si>
+    <t>Standardized parameters for the property.</t>
+  </si>
+  <si>
+    <t>VC+HIP+A</t>
+  </si>
+  <si>
+    <t>BCC+FCC+2?</t>
+  </si>
+  <si>
+    <t>MaxStress 120e6 Pa, …</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>BCC+FCC</t>
+  </si>
+  <si>
+    <t>HIP+A</t>
+  </si>
+  <si>
+    <t>UTS</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Fe60 Ni10 Cr20 Zr10</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Fe60 Ni10 Cr10 Zr20</t>
+  </si>
+  <si>
+    <t>3BCC+MC</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Fe25 Ni25 Cr25 Zr25</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>FeNiCrZr</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Ti0.1 (ZrHfNb)0.3</t>
+  </si>
+  <si>
+    <t>FCC</t>
+  </si>
+  <si>
+    <t>EMP</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Fe0.60 Ni0.10 Cr0.10 Zr0.20</t>
+  </si>
+  <si>
+    <t>BCC+2?</t>
+  </si>
+  <si>
+    <t>SPS</t>
+  </si>
+  <si>
+    <t>THM</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>cast from 2000K</t>
+  </si>
+  <si>
+    <t>CreepRate</t>
+  </si>
+  <si>
+    <t>MaxStress 80e6 Pa</t>
+  </si>
+  <si>
+    <t>s-1</t>
+  </si>
+  <si>
+    <t>Sun_2022_CreepRatePredictions</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>W90 Mo5 Ti5</t>
+  </si>
+  <si>
+    <t>3?+laves</t>
+  </si>
+  <si>
+    <t>BCT+laves</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>annealed for 48h at 1600K</t>
+  </si>
+  <si>
+    <t>HfMoNbZrTiCrAlW</t>
+  </si>
+  <si>
+    <t>BCC+?+?+?</t>
+  </si>
+  <si>
+    <t>UTS_Arindam_v0.7.4</t>
+  </si>
+  <si>
+    <t>popular abbreviation or "full property name"</t>
+  </si>
+  <si>
+    <t>Absolute Temperature [K]</t>
   </si>
   <si>
     <r>
@@ -143,7 +350,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>able</t>
+      <t xml:space="preserve">able </t>
     </r>
     <r>
       <rPr>
@@ -153,7 +360,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/F</t>
+      <t>/ F</t>
     </r>
     <r>
       <rPr>
@@ -163,7 +370,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>igure</t>
+      <t xml:space="preserve">igure </t>
     </r>
     <r>
       <rPr>
@@ -173,7 +380,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/A</t>
+      <t>/ A</t>
     </r>
     <r>
       <rPr>
@@ -193,7 +400,25 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> S</t>
+      <t xml:space="preserve"> P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>age</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / S</t>
     </r>
     <r>
       <rPr>
@@ -207,221 +432,17 @@
     </r>
   </si>
   <si>
-    <t>id/nickname</t>
-  </si>
-  <si>
-    <t>Optional Upload Comments:</t>
-  </si>
-  <si>
-    <t>popular abbreviation or FullPropertyName</t>
-  </si>
-  <si>
-    <t>750e6</t>
-  </si>
-  <si>
-    <t>Col1</t>
-  </si>
-  <si>
-    <t>Col2</t>
-  </si>
-  <si>
-    <t>Col3</t>
-  </si>
-  <si>
-    <t>Col4</t>
-  </si>
-  <si>
-    <t>Col5</t>
-  </si>
-  <si>
-    <t>Scratch (NOT UPLOADED)</t>
-  </si>
-  <si>
-    <t>UTS in lb/in^2</t>
-  </si>
-  <si>
-    <t>Temperature in F</t>
-  </si>
-  <si>
-    <t>Some Notes</t>
-  </si>
-  <si>
-    <t>only DOI, no http etc                                                      (if no DOI) Author_Year_ThreeFirstTitleWords</t>
-  </si>
-  <si>
-    <t>Pa</t>
-  </si>
-  <si>
-    <t>Unit [SI]</t>
-  </si>
-  <si>
-    <t>Uncertainty in Value</t>
-  </si>
-  <si>
-    <t>25e6</t>
-  </si>
-  <si>
-    <t>Uncertainty [SI]</t>
-  </si>
-  <si>
-    <t>Special Cell</t>
-  </si>
-  <si>
-    <t>This special cell will allow running special upload functions in the future, such as (1) POSCAR, (2) TDB, (3) FIGURE, by typing the word In the cell below to engage upload script function</t>
-  </si>
-  <si>
-    <t>Property Parameters</t>
-  </si>
-  <si>
-    <t>Standardized parameters for the property.</t>
-  </si>
-  <si>
-    <t>UTS / CreepRate</t>
-  </si>
-  <si>
-    <t>VC+HIP+A</t>
-  </si>
-  <si>
-    <t>BCC+FCC+2?</t>
-  </si>
-  <si>
-    <t>MaxStress 120e6 Pa, …</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>BCC+FCC</t>
-  </si>
-  <si>
-    <t>HIP+A</t>
-  </si>
-  <si>
-    <t>UTS</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Fe60 Ni10 Cr20 Zr10</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Fe60 Ni10 Cr10 Zr20</t>
-  </si>
-  <si>
-    <t>3BCC+MC</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Fe25 Ni25 Cr25 Zr25</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>FeNiCrZr</t>
-  </si>
-  <si>
-    <t>BCC</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>ML</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Ti0.1 (ZrHfNb)0.3</t>
-  </si>
-  <si>
-    <t>FCC</t>
-  </si>
-  <si>
-    <t>EMP</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Fe0.60 Ni0.10 Cr0.10 Zr0.20</t>
-  </si>
-  <si>
-    <t>BCC+2?</t>
-  </si>
-  <si>
-    <t>SPS</t>
-  </si>
-  <si>
-    <t>THM</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>cast from 2000K</t>
-  </si>
-  <si>
-    <t>CreepRate</t>
-  </si>
-  <si>
-    <t>MaxStress 80e6 Pa</t>
-  </si>
-  <si>
-    <t>s-1</t>
-  </si>
-  <si>
-    <t>Sun_2022_CreepRatePredictions</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>W90 Mo5 Ti5</t>
-  </si>
-  <si>
-    <t>3?+laves</t>
-  </si>
-  <si>
-    <t>BCT+laves</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>annealed for 48h at 1600K</t>
-  </si>
-  <si>
-    <t>HfMoNbZrTiCrAlW</t>
-  </si>
-  <si>
-    <t>BCC+?+?+?</t>
-  </si>
-  <si>
-    <t>UTS_Arindam_v0.7.4</t>
+    <t>UTS / creep rate</t>
+  </si>
+  <si>
+    <t>T7 / F6 / P13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,6 +522,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1098,33 +1124,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1174,6 +1173,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1460,15 +1486,14 @@
   <dimension ref="A1:T430"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="6" width="17.83203125" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
@@ -1477,7 +1502,8 @@
     <col min="11" max="11" width="15.33203125" customWidth="1"/>
     <col min="12" max="12" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="17.83203125" customWidth="1"/>
-    <col min="14" max="15" width="39.33203125" customWidth="1"/>
+    <col min="14" max="14" width="34.6640625" customWidth="1"/>
+    <col min="15" max="15" width="39.33203125" customWidth="1"/>
     <col min="16" max="16" width="17.6640625" customWidth="1"/>
     <col min="17" max="18" width="18" customWidth="1"/>
     <col min="19" max="20" width="17.5" customWidth="1"/>
@@ -1495,19 +1521,19 @@
       <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="51"/>
+      <c r="D2" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="46"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
       <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1517,17 +1543,17 @@
       <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="53"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1545,66 +1571,66 @@
       <c r="B5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="47" t="s">
+      <c r="C5" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="D5" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="47" t="s">
+      <c r="F5" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="47" t="s">
+      <c r="H5" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="47" t="s">
+      <c r="K5" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="O5" s="41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="N5" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="42"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="60"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1614,87 +1640,87 @@
         <v>20</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I7" s="6">
         <v>298</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="43"/>
+      <c r="O7" s="61"/>
       <c r="P7" s="33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R7" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61" t="s">
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="64" t="s">
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="65"/>
+      <c r="N8" s="56"/>
       <c r="O8" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="P8" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="46"/>
+        <v>52</v>
+      </c>
+      <c r="P8" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="64"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>9</v>
@@ -1715,7 +1741,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>22</v>
@@ -1724,10 +1750,10 @@
         <v>23</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M9" s="28" t="s">
         <v>17</v>
@@ -1737,39 +1763,39 @@
       </c>
       <c r="O9" s="32"/>
       <c r="P9" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q9" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="23" t="s">
+      <c r="T9" s="24" t="s">
         <v>41</v>
-      </c>
-      <c r="R9" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="S9" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="T9" s="24" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G10" s="35" t="s">
         <v>21</v>
@@ -1785,7 +1811,7 @@
         <v>25000000</v>
       </c>
       <c r="L10" s="36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M10" s="35" t="s">
         <v>25</v>
@@ -1797,22 +1823,22 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G11" s="35" t="s">
         <v>21</v>
@@ -1828,7 +1854,7 @@
         <v>25000000</v>
       </c>
       <c r="L11" s="36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M11" s="35" t="s">
         <v>25</v>
@@ -1840,22 +1866,22 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G12" s="35" t="s">
         <v>21</v>
@@ -1871,7 +1897,7 @@
         <v>25000000</v>
       </c>
       <c r="L12" s="36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M12" s="35" t="s">
         <v>25</v>
@@ -1883,22 +1909,22 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G13" s="35" t="s">
         <v>21</v>
@@ -1914,7 +1940,7 @@
         <v>25000000</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M13" s="35" t="s">
         <v>25</v>
@@ -1926,26 +1952,26 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E14" s="35"/>
       <c r="F14" s="35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I14" s="39">
         <v>298</v>
@@ -1955,7 +1981,7 @@
       </c>
       <c r="K14" s="34"/>
       <c r="L14" s="36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M14" s="35" t="s">
         <v>25</v>
@@ -1967,23 +1993,23 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H15" s="35"/>
       <c r="I15" s="39">
@@ -1996,7 +2022,7 @@
         <v>10000000</v>
       </c>
       <c r="L15" s="36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M15" s="35"/>
       <c r="N15" s="21"/>
@@ -2004,23 +2030,23 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H16" s="35"/>
       <c r="I16" s="39">
@@ -2033,10 +2059,10 @@
         <v>50000000</v>
       </c>
       <c r="L16" s="36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M16" s="35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N16" s="21" t="s">
         <v>26</v>
@@ -2045,28 +2071,28 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>93</v>
-      </c>
       <c r="G17" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I17" s="39">
         <v>298</v>
@@ -2078,27 +2104,27 @@
         <v>1E-8</v>
       </c>
       <c r="L17" s="40" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M17" s="40" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="35"/>
@@ -2113,16 +2139,16 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="35"/>
@@ -8244,6 +8270,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -8258,11 +8289,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>

</xml_diff>